<commit_message>
Updated main and new xlsx files
</commit_message>
<xml_diff>
--- a/mesh_16_m5out_stats.xlsx
+++ b/mesh_16_m5out_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\soliman\m5out_stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F08E1F-688A-4439-9552-D6FB575478E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420F10D6-77DF-4787-B166-D6E066F3368B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1095,12 +1095,13 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>